<commit_message>
- Flow updated for the donwloaded files to be saved in the default "Downloads" folder - Flow updated to move the downloaded files from the "Downloads" folder to the MasterFolder
</commit_message>
<xml_diff>
--- a/IRConfigFile.xlsx
+++ b/IRConfigFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\IRCRUOps_ReportMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2389AFD1-8E1A-4D56-9B4B-317E2DBA42BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406DEAAF-8075-4489-A1E4-ED5111C7C6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -168,13 +168,19 @@
     <t>https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FPA%20HP%2F</t>
   </si>
   <si>
-    <t>DONE&amp;viewid=0cafe987%2D9ce0%2D4c52%2Dbaeb%2D28681de003dc</t>
-  </si>
-  <si>
-    <t>Lester.Rollan@lexisnexisrisk.com; Dindee.Galindo@lexisnexisrisk.com; Jomar.Espos@lexisnexisrisk.com; Jhoanna.Talle@lexisnexisrisk.com; ELMERA.BALBONA@lexisnexisrisk.com</t>
-  </si>
-  <si>
-    <t>Jann.Orbe@lexisnexisrisk.com; Jesriel.Tolentino@lexisnexisrisk.com; Sam.Tecson@lexisnexisrisk.com; Joavic.Quisano@lexisnexisrisk.com</t>
+    <t>Lester.Rollan@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>DownloadsFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\svc-RCOUIPBOT0005\Downloads\</t>
+  </si>
+  <si>
+    <t>Download folder's path</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\Downloads\</t>
   </si>
 </sst>
 </file>
@@ -608,18 +614,18 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.81640625" style="2"/>
+    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -630,7 +636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -641,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -652,7 +658,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -663,7 +669,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -674,7 +680,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -685,7 +691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -696,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -707,7 +713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -718,71 +724,77 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
+      <c r="B10" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>44</v>
+      <c r="B11" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="B14" s="5"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FPA%20HP%2F" xr:uid="{757D07F4-6C5F-4570-B732-0325875F2960}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{A58EE4EF-599E-4D8A-8380-6462F59B612E}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{79646B93-E09A-4925-9D5A-BC87FECEB893}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -792,25 +804,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="78.81640625" customWidth="1"/>
-    <col min="3" max="3" width="64.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -821,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -832,7 +844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -843,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -854,7 +866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -865,7 +877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -876,7 +888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -887,7 +899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -898,7 +910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -909,7 +921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -920,7 +932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -931,24 +943,30 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -959,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -970,7 +988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -981,7 +999,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -992,7 +1010,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1003,7 +1021,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1014,7 +1032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1036,7 +1054,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1047,7 +1065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -1058,7 +1076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1069,14 +1087,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1098,7 +1127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1120,7 +1149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1142,7 +1171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -1153,7 +1182,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
@@ -1164,7 +1193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>27</v>
       </c>
@@ -1175,7 +1204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
@@ -1186,7 +1215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -1197,7 +1226,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit and push to new repository
</commit_message>
<xml_diff>
--- a/IRConfigFile.xlsx
+++ b/IRConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\IRCRUOps_ReportMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406DEAAF-8075-4489-A1E4-ED5111C7C6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDC0096-0C75-47DE-9C1C-E485541A37D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FPA%20HP%2F</t>
   </si>
   <si>
-    <t>Lester.Rollan@lexisnexisrisk.com</t>
-  </si>
-  <si>
     <t>DownloadsFolder</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>C:\Users\RollLe01\Downloads\</t>
+  </si>
+  <si>
+    <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B16" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,19 +728,19 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>43</v>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>43</v>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -748,13 +748,13 @@
     </row>
     <row r="12" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,8 +793,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FPA%20HP%2F" xr:uid="{757D07F4-6C5F-4570-B732-0325875F2960}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{A58EE4EF-599E-4D8A-8380-6462F59B612E}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{79646B93-E09A-4925-9D5A-BC87FECEB893}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -804,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,13 +943,13 @@
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,13 +1087,13 @@
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,15 +1224,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>